<commit_message>
further describing relatino extractor
</commit_message>
<xml_diff>
--- a/graphs/Workbook1.xlsx
+++ b/graphs/Workbook1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16180" tabRatio="500"/>
   </bookViews>
@@ -581,11 +581,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124157784"/>
-        <c:axId val="-2124155608"/>
+        <c:axId val="-2123060504"/>
+        <c:axId val="-2122582664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2124157784"/>
+        <c:axId val="-2123060504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,7 +604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2124155608"/>
+        <c:crossAx val="-2122582664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -612,7 +612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124155608"/>
+        <c:axId val="-2122582664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -623,16 +623,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124157784"/>
+        <c:crossAx val="-2123060504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1004,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C7:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>